<commit_message>
Fixes a math error in indst/TNRbI
</commit_message>
<xml_diff>
--- a/InputData/indst/TNRbI/Total Nonfuel Revenue by Industry.xlsx
+++ b/InputData/indst/TNRbI/Total Nonfuel Revenue by Industry.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\Dropbox\EPS India 2.1 - Input Data Revisions_17Mar2020\TNRbI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\India\Models\eps-india\InputData\indst\TNRbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391C7712-0A3C-43F6-9548-18D2F68AD264}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
     <definedName name="currency_conv">About!#REF!</definedName>
     <definedName name="Preferences.moneyunits">[1]Preferences!$C$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -839,12 +838,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -1243,10 +1242,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1255,7 +1254,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -1265,7 +1264,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1293,7 +1292,7 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -1330,7 +1329,7 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1346,12 +1345,12 @@
     <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="19" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1375,10 +1374,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1389,19 +1388,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Body: normal cell" xfId="5"/>
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Header: bottom row" xfId="6" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="7"/>
+    <cellStyle name="Footnotes: top row" xfId="3"/>
+    <cellStyle name="Header: bottom row" xfId="6"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal_Template-EUKLEMS-output" xfId="10" xr:uid="{7EDA8E80-0E11-4A3A-A263-57863A888204}"/>
-    <cellStyle name="Parent row" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Table title" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal_Template-EUKLEMS-output" xfId="10"/>
+    <cellStyle name="Parent row" xfId="4"/>
+    <cellStyle name="Table title" xfId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1631,23 +1632,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1683,23 +1667,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1875,11 +1842,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,7 +2151,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6964,7 +6931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179C9E4E-4AB6-48A2-8A45-F5D4B8DF8998}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7923,11 +7890,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E565CA86-C912-4881-8020-A2529820D8D2}">
-  <dimension ref="A1:G29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7938,14 +7905,16 @@
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>156</v>
       </c>
@@ -7968,7 +7937,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="44">
         <v>1</v>
       </c>
@@ -7993,8 +7962,16 @@
         <f>F3*About!$B$54</f>
         <v>469134281564.11652</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="68">
+        <f>D3*10000000</f>
+        <v>32014900000000</v>
+      </c>
+      <c r="I3" s="69">
+        <f>H3*0.014</f>
+        <v>448208600000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="44">
         <v>2</v>
       </c>
@@ -8020,7 +7997,7 @@
         <v>82724099082.424347</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="44">
         <v>3</v>
       </c>
@@ -8046,7 +8023,7 @@
         <v>178625175759.99658</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="44">
         <v>4</v>
       </c>
@@ -8072,7 +8049,7 @@
         <v>145713870721.43866</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="44">
         <v>5</v>
       </c>
@@ -8098,7 +8075,7 @@
         <v>13194122334.29842</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="44">
         <v>6</v>
       </c>
@@ -8124,7 +8101,7 @@
         <v>26568777306.48951</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="44">
         <v>7</v>
       </c>
@@ -8150,7 +8127,7 @@
         <v>203030052527.71906</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="44">
         <v>8</v>
       </c>
@@ -8176,7 +8153,7 @@
         <v>158444498953.74481</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="44">
         <v>9</v>
       </c>
@@ -8202,7 +8179,7 @@
         <v>40649150772.261017</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="44">
         <v>10</v>
       </c>
@@ -8228,7 +8205,7 @@
         <v>49407914434.696442</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="44">
         <v>11</v>
       </c>
@@ -8254,7 +8231,7 @@
         <v>187479769440.06223</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="44">
         <v>12</v>
       </c>
@@ -8280,7 +8257,7 @@
         <v>65365061252.617935</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="44">
         <v>13</v>
       </c>
@@ -8306,7 +8283,7 @@
         <v>63448435769.535637</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="44">
         <v>14</v>
       </c>
@@ -8676,7 +8653,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB845EF-5FB2-4C6C-A558-C90A8D2382EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8759,8 +8736,8 @@
         <v>11</v>
       </c>
       <c r="B8" s="52">
-        <f>'India KLEMS DB'!G3*70</f>
-        <v>32839399709488.156</v>
+        <f>'India KLEMS DB'!G3*0.7</f>
+        <v>328393997094.88153</v>
       </c>
       <c r="C8" s="54" t="s">
         <v>255</v>
@@ -8784,14 +8761,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9633,135 +9610,135 @@
       </c>
       <c r="B8" s="26">
         <f>'Start Year Values'!B8</f>
-        <v>32839399709488.156</v>
+        <v>328393997094.88153</v>
       </c>
       <c r="C8" s="26">
         <f>B8*(1+'IESS growth rates'!$L$8)</f>
-        <v>33069275507454.57</v>
+        <v>330692755074.54565</v>
       </c>
       <c r="D8" s="26">
         <f>C8*(1+'IESS growth rates'!$L$8)</f>
-        <v>33300760436006.75</v>
+        <v>333007604360.06744</v>
       </c>
       <c r="E8" s="26">
         <f>D8*(1+'IESS growth rates'!$L$8)</f>
-        <v>33533865759058.793</v>
+        <v>335338657590.58789</v>
       </c>
       <c r="F8" s="26">
         <f>E8*(1+'IESS growth rates'!$L$8)</f>
-        <v>33768602819372.199</v>
+        <v>337686028193.72198</v>
       </c>
       <c r="G8" s="26">
         <f>F8*(1+'IESS growth rates'!$M$8)</f>
-        <v>33937445833469.055</v>
+        <v>339374458334.69055</v>
       </c>
       <c r="H8" s="26">
         <f>G8*(1+'IESS growth rates'!$M$8)</f>
-        <v>34107133062636.395</v>
+        <v>341071330626.36395</v>
       </c>
       <c r="I8" s="26">
         <f>H8*(1+'IESS growth rates'!$M$8)</f>
-        <v>34277668727949.574</v>
+        <v>342776687279.49573</v>
       </c>
       <c r="J8" s="26">
         <f>I8*(1+'IESS growth rates'!$M$8)</f>
-        <v>34449057071589.32</v>
+        <v>344490570715.89319</v>
       </c>
       <c r="K8" s="26">
         <f>J8*(1+'IESS growth rates'!$M$8)</f>
-        <v>34621302356947.262</v>
+        <v>346213023569.4726</v>
       </c>
       <c r="L8" s="26">
         <f>K8*(1+'IESS growth rates'!$M$8)</f>
-        <v>34794408868731.996</v>
+        <v>347944088687.31995</v>
       </c>
       <c r="M8" s="26">
         <f>L8*(1+'IESS growth rates'!$M$8)</f>
-        <v>34968380913075.652</v>
+        <v>349683809130.75653</v>
       </c>
       <c r="N8" s="26">
         <f>M8*(1+'IESS growth rates'!$M$8)</f>
-        <v>35143222817641.027</v>
+        <v>351432228176.41028</v>
       </c>
       <c r="O8" s="26">
         <f>N8*(1+'IESS growth rates'!$M$8)</f>
-        <v>35318938931729.227</v>
+        <v>353189389317.2923</v>
       </c>
       <c r="P8" s="26">
         <f>O8*(1+'IESS growth rates'!$M$8)</f>
-        <v>35495533626387.867</v>
+        <v>354955336263.87872</v>
       </c>
       <c r="Q8" s="26">
         <f>P8*(1+'IESS growth rates'!$N$8)</f>
-        <v>35584272460453.836</v>
+        <v>355842724604.53839</v>
       </c>
       <c r="R8" s="26">
         <f>Q8*(1+'IESS growth rates'!$N$8)</f>
-        <v>35673233141604.969</v>
+        <v>356732331416.04974</v>
       </c>
       <c r="S8" s="26">
         <f>R8*(1+'IESS growth rates'!$N$8)</f>
-        <v>35762416224458.977</v>
+        <v>357624162244.58984</v>
       </c>
       <c r="T8" s="26">
         <f>S8*(1+'IESS growth rates'!$N$8)</f>
-        <v>35851822265020.125</v>
+        <v>358518222650.20129</v>
       </c>
       <c r="U8" s="26">
         <f>T8*(1+'IESS growth rates'!$N$8)</f>
-        <v>35941451820682.672</v>
+        <v>359414518206.82678</v>
       </c>
       <c r="V8" s="26">
         <f>U8*(1+'IESS growth rates'!$N$8)</f>
-        <v>36031305450234.375</v>
+        <v>360313054502.34381</v>
       </c>
       <c r="W8" s="26">
         <f>V8*(1+'IESS growth rates'!$N$8)</f>
-        <v>36121383713859.961</v>
+        <v>361213837138.59967</v>
       </c>
       <c r="X8" s="26">
         <f>W8*(1+'IESS growth rates'!$N$8)</f>
-        <v>36211687173144.609</v>
+        <v>362116871731.44617</v>
       </c>
       <c r="Y8" s="26">
         <f>X8*(1+'IESS growth rates'!$N$8)</f>
-        <v>36302216391077.469</v>
+        <v>363022163910.77478</v>
       </c>
       <c r="Z8" s="26">
         <f>Y8*(1+'IESS growth rates'!$N$8)</f>
-        <v>36392971932055.164</v>
+        <v>363929719320.5517</v>
       </c>
       <c r="AA8" s="26">
         <f>Z8*(1+'IESS growth rates'!$O$8)</f>
-        <v>36447561389953.25</v>
+        <v>364475613899.53253</v>
       </c>
       <c r="AB8" s="26">
         <f>AA8*(1+'IESS growth rates'!$O$8)</f>
-        <v>36502232732038.18</v>
+        <v>365022327320.38184</v>
       </c>
       <c r="AC8" s="26">
         <f>AB8*(1+'IESS growth rates'!$O$8)</f>
-        <v>36556986081136.242</v>
+        <v>365569860811.36243</v>
       </c>
       <c r="AD8" s="26">
         <f>AC8*(1+'IESS growth rates'!$O$8)</f>
-        <v>36611821560257.945</v>
+        <v>366118215602.57947</v>
       </c>
       <c r="AE8" s="26">
         <f>AD8*(1+'IESS growth rates'!$O$8)</f>
-        <v>36666739292598.336</v>
+        <v>366667392925.98334</v>
       </c>
       <c r="AF8" s="26">
         <f>AE8*(1+'IESS growth rates'!$O$8)</f>
-        <v>36721739401537.234</v>
+        <v>367217394015.37231</v>
       </c>
       <c r="AG8" s="26">
         <f>AF8*(1+'IESS growth rates'!$O$8)</f>
-        <v>36776822010639.539</v>
+        <v>367768220106.39539</v>
       </c>
       <c r="AH8" s="26">
         <f>AG8*(1+'IESS growth rates'!$O$8)</f>
-        <v>36831987243655.5</v>
+        <v>368319872436.55499</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">

</xml_diff>